<commit_message>
add stage json map
</commit_message>
<xml_diff>
--- a/Sprite/sprites.xlsx
+++ b/Sprite/sprites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\00.project\02.SmartphoneGameProgramming\AndroidGameProgramming\Sprite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AE47D68-F907-4C62-B14C-80385F92D1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B752BF-8F55-4BD6-BBD4-FBCE75D5644C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{932CE131-C182-49D1-8CB0-9AFDD0C5ADB7}"/>
   </bookViews>
@@ -108,9 +108,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>289034</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>289034</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -126,7 +126,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1143000" cy="466725"/>
+          <a:ext cx="578068" cy="289034"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -179,16 +179,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1142999</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>289034</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2295524</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>289033</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>289034</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -203,8 +203,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1142999" y="0"/>
-          <a:ext cx="2295525" cy="466725"/>
+          <a:off x="578068" y="0"/>
+          <a:ext cx="867103" cy="289034"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -257,16 +257,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>289034</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -281,8 +281,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1752600" y="352425"/>
-          <a:ext cx="685800" cy="285750"/>
+          <a:off x="1445172" y="0"/>
+          <a:ext cx="289035" cy="289035"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -335,16 +335,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>289034</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>289033</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -359,8 +359,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2042948" y="643759"/>
-          <a:ext cx="1228397" cy="2384534"/>
+          <a:off x="1734206" y="1"/>
+          <a:ext cx="867103" cy="1445172"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -413,16 +413,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>289033</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -437,8 +437,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3271345" y="643759"/>
-          <a:ext cx="1241534" cy="2384534"/>
+          <a:off x="2601309" y="1"/>
+          <a:ext cx="578070" cy="1445172"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -491,16 +491,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>289033</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289033</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -515,8 +515,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4512879" y="643759"/>
-          <a:ext cx="1241535" cy="2384534"/>
+          <a:off x="3179378" y="1"/>
+          <a:ext cx="867103" cy="1445172"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -569,14 +569,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>289033</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -593,14 +593,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5754415" y="3028293"/>
-          <a:ext cx="1885292" cy="1721069"/>
+          <a:off x="4046483" y="0"/>
+          <a:ext cx="1445171" cy="1156138"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:blipFill dpi="0" rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                 <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -948,31 +948,26 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G4"/>
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="3.75" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
-    <col min="5" max="6" width="16.25" customWidth="1"/>
-    <col min="7" max="7" width="24.75" customWidth="1"/>
+    <col min="1" max="33" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" ht="187.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" ht="126" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" ht="36.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>